<commit_message>
Update to DataDict templates 09022020
Update to DataDict templates 09022020.  Small changes.
</commit_message>
<xml_diff>
--- a/DataDict/Aggregate/Template_basin_aggregate_data_dictionary_WaDE_August2020_v1.xlsx
+++ b/DataDict/Aggregate/Template_basin_aggregate_data_dictionary_WaDE_August2020_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\DataDict\Aggregate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A33ED64-76B0-4176-9982-314B9AFE31B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467442CB-663F-4B07-AE8B-7D9D57CBDD7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{72C05CBC-82A9-4295-85A4-76EE06FFC478}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{72C05CBC-82A9-4295-85A4-76EE06FFC478}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="10" r:id="rId1"/>
@@ -942,116 +942,116 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1437,7 +1437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2403CCCD-12BC-4468-8E1E-FDDA82B7D922}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1448,42 +1448,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1582,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530E092E-37FC-44C0-9387-B111C2DA4E7B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1596,29 +1596,29 @@
     <col min="8" max="8" width="26.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="53" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:8" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="51" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1648,29 +1648,29 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+    <row r="3" spans="1:8" s="57" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="57" t="s">
+      <c r="H3" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1694,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E08C38F-342B-49D5-9FE3-F27BCCD90258}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1710,29 +1710,29 @@
     <col min="8" max="8" width="18.6640625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="53" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:8" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="49" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1762,11 +1762,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="62" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="61" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="59" t="s">
         <v>102</v>
       </c>
       <c r="C3" s="47">
@@ -1784,7 +1784,7 @@
       <c r="G3" s="47">
         <v>10</v>
       </c>
-      <c r="H3" s="61" t="s">
+      <c r="H3" s="60" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85242FD5-FD52-4C86-8C01-7E742284680E}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1822,23 +1822,23 @@
     <col min="7" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="51" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1862,23 +1862,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="64" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="63">
+    <row r="3" spans="1:6" s="63" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="62">
         <v>17839</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="56" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1899,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F72A969-622D-4936-987A-049101D32A6E}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1916,29 +1916,29 @@
     <col min="9" max="9" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="53" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:8" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="51" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1968,8 +1968,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="68" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:8" s="67" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="59" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -1981,16 +1981,16 @@
       <c r="D3" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="66">
+      <c r="E3" s="65">
         <v>0.5</v>
       </c>
-      <c r="F3" s="69">
+      <c r="F3" s="68">
         <v>0.9</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="66" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57FC1D5-7413-4D4B-8F4B-A0DAC5C798A1}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2030,29 +2030,29 @@
     <col min="9" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2082,29 +2082,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="75" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72">
+    <row r="3" spans="1:8" s="74" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="71">
         <v>3703994</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="72">
         <v>1</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF95F0A-A6D8-4C9F-9AAD-CE9D64114AA9}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D13" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
@@ -2158,62 +2158,62 @@
     <col min="19" max="19" width="29.88671875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="53" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:19" s="52" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="79" t="s">
+      <c r="J1" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="79" t="s">
+      <c r="L1" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="79" t="s">
+      <c r="N1" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="79" t="s">
+      <c r="O1" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="Q1" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="79" t="s">
+      <c r="R1" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="79" t="s">
+      <c r="S1" s="78" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2276,62 +2276,62 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="75" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="82">
+    <row r="3" spans="1:19" s="74" customFormat="1" ht="10.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="81">
         <v>1200</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="80" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="83">
+      <c r="F3" s="82">
         <v>2533</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="66">
+      <c r="I3" s="65">
         <v>0.15</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="66">
+      <c r="M3" s="65">
         <v>20</v>
       </c>
-      <c r="N3" s="66" t="s">
+      <c r="N3" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="O3" s="84" t="s">
+      <c r="O3" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="80" t="s">
+      <c r="P3" s="79" t="s">
         <v>143</v>
       </c>
-      <c r="Q3" s="66" t="s">
+      <c r="Q3" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="R3" s="66">
+      <c r="R3" s="65">
         <v>2012</v>
       </c>
-      <c r="S3" s="84" t="s">
+      <c r="S3" s="83" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>